<commit_message>
Marco teorico casi terminado
</commit_message>
<xml_diff>
--- a/Docs/Excel de datos.xlsx
+++ b/Docs/Excel de datos.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TFG\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F8302E-4959-4D86-B7BC-49B764ED5BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E58AAA-B1E5-4568-B2A6-402D94C587CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="5640" windowWidth="28800" windowHeight="15345" xr2:uid="{3B9EF640-BB6A-4E7B-9EC3-AD66720BE4AC}"/>
+    <workbookView xWindow="38280" yWindow="-3750" windowWidth="16440" windowHeight="28320" xr2:uid="{3B9EF640-BB6A-4E7B-9EC3-AD66720BE4AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="44">
   <si>
     <t>HOMBRES</t>
   </si>
@@ -308,7 +307,7 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4356,6 +4355,1714 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>33% &lt;= GDF &lt; 45%</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>   </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>                                       </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>45% &lt;= GDF &lt; 64%</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>                               </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>64% &lt;= GDF &lt; 75%</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>                                               </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>GDF &gt;=75%</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES" sz="900" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12474452568233772"/>
+          <c:y val="0.93264529903591331"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$143</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Menos de 7 años</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$144:$A$151</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$144:$B$151</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>15227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7217</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2539</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1348</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1479</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1146</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>905</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6011-4385-80BA-9FC523853FA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$143</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>De 7 a 17 años</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$144:$A$151</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$144:$C$151</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>57712</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26260</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13254</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7067</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8978</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5221</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7784</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6011-4385-80BA-9FC523853FA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$143</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>De 18 a 34 años</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$144:$A$151</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$144:$D$151</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>57601</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39532</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18685</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12939</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32724</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21749</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24309</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17169</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6011-4385-80BA-9FC523853FA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$E$143</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>De 35 a 64 años</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$144:$A$151</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$E$144:$E$151</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>334891</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>291944</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124679</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>118754</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>192394</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>162624</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91939</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74578</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6011-4385-80BA-9FC523853FA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$F$143</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>De 65 a 79 años</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$144:$A$151</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$F$144:$F$151</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>199316</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>174511</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97367</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91170</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>115626</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54840</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6011-4385-80BA-9FC523853FA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$G$143</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> De 80 años o más</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$144:$A$151</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hombres</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mujeres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$G$144:$G$151</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>70706</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78404</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38291</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51544</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>107488</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57813</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125389</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-6011-4385-80BA-9FC523853FA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="730865663"/>
+        <c:axId val="730866079"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="730865663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="730866079"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="730866079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="730865663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11720469916278223"/>
+          <c:y val="0.97004369455730599"/>
+          <c:w val="0.78125632650795263"/>
+          <c:h val="2.9956305442694009E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$133</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Menos de 7 años</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$134:$A$141</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$134:$B$141</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>15227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7217</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2539</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1348</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1479</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1146</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>905</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6130-4D87-9D5C-A0EA1501DE16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$133</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>De 7 a 17 años</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$134:$A$141</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$134:$C$141</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>57712</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26260</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13254</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7067</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8978</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5221</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7784</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6130-4D87-9D5C-A0EA1501DE16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$133</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>De 18 a 34 años</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$134:$A$141</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$134:$D$141</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>57601</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39532</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18685</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12939</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32724</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21749</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24309</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17169</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6130-4D87-9D5C-A0EA1501DE16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$E$133</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>De 35 a 64 años</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$134:$A$141</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$E$134:$E$141</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>334891</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>291944</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124679</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>118754</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>192394</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>162624</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91939</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74578</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6130-4D87-9D5C-A0EA1501DE16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$F$133</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>De 65 a 79 años</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$134:$A$141</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$F$134:$F$141</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>199316</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>174511</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97367</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91170</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>115626</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54840</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6130-4D87-9D5C-A0EA1501DE16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$G$133</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> De 80 años o más</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$134:$A$141</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33% &lt;= GDF &lt; 45%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45% &lt;= GDF &lt; 64%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64% &lt;= GDF &lt; 75%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>GDF &gt;=75%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$G$134:$G$141</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>70706</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78404</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38291</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51544</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>107488</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57813</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125389</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-6130-4D87-9D5C-A0EA1501DE16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="887015839"/>
+        <c:axId val="887016255"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="887015839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="887016255"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="887016255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="887015839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4596,6 +6303,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -7324,6 +9111,1016 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -7884,6 +10681,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1461383</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>103197</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>661283</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>165434</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{681091E7-2E52-D3BC-0EBF-38C11D5E5CE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>645502</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>36999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>388327</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>32238</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D93EA046-6E6E-197C-9901-71A13CF8C125}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8184,9 +11053,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BAE422-1974-4CCE-8B1E-2F921F086639}">
-  <dimension ref="A1:M151"/>
+  <dimension ref="A1:T166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
@@ -8197,7 +11066,7 @@
     <col min="3" max="3" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
@@ -9167,8 +12036,212 @@
         <v>523966</v>
       </c>
     </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G133" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B134" s="17">
+        <v>15227</v>
+      </c>
+      <c r="C134" s="16">
+        <v>57712</v>
+      </c>
+      <c r="D134" s="16">
+        <v>57601</v>
+      </c>
+      <c r="E134" s="16">
+        <v>334891</v>
+      </c>
+      <c r="F134" s="16">
+        <v>199316</v>
+      </c>
+      <c r="G134" s="16">
+        <v>70706</v>
+      </c>
+    </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B135" s="21"/>
+      <c r="A135" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B135" s="14">
+        <v>7217</v>
+      </c>
+      <c r="C135" s="14">
+        <v>26260</v>
+      </c>
+      <c r="D135" s="14">
+        <v>39532</v>
+      </c>
+      <c r="E135" s="14">
+        <v>291944</v>
+      </c>
+      <c r="F135" s="14">
+        <v>174511</v>
+      </c>
+      <c r="G135" s="14">
+        <v>78404</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B136" s="8">
+        <v>2539</v>
+      </c>
+      <c r="C136" s="8">
+        <v>13254</v>
+      </c>
+      <c r="D136" s="8">
+        <v>18685</v>
+      </c>
+      <c r="E136" s="8">
+        <v>124679</v>
+      </c>
+      <c r="F136" s="8">
+        <v>85666</v>
+      </c>
+      <c r="G136" s="8">
+        <v>38291</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B137" s="8">
+        <v>1348</v>
+      </c>
+      <c r="C137" s="8">
+        <v>7067</v>
+      </c>
+      <c r="D137" s="8">
+        <v>12939</v>
+      </c>
+      <c r="E137" s="8">
+        <v>118754</v>
+      </c>
+      <c r="F137" s="8">
+        <v>97367</v>
+      </c>
+      <c r="G137" s="8">
+        <v>65973</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B138" s="14">
+        <v>1479</v>
+      </c>
+      <c r="C138" s="14">
+        <v>8978</v>
+      </c>
+      <c r="D138" s="14">
+        <v>32724</v>
+      </c>
+      <c r="E138" s="14">
+        <v>192394</v>
+      </c>
+      <c r="F138" s="14">
+        <v>91170</v>
+      </c>
+      <c r="G138" s="14">
+        <v>51544</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B139" s="10">
+        <v>997</v>
+      </c>
+      <c r="C139" s="14">
+        <v>5221</v>
+      </c>
+      <c r="D139" s="14">
+        <v>21749</v>
+      </c>
+      <c r="E139" s="14">
+        <v>162624</v>
+      </c>
+      <c r="F139" s="14">
+        <v>115626</v>
+      </c>
+      <c r="G139" s="14">
+        <v>107488</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B140" s="8">
+        <v>1146</v>
+      </c>
+      <c r="C140" s="8">
+        <v>7784</v>
+      </c>
+      <c r="D140" s="8">
+        <v>24309</v>
+      </c>
+      <c r="E140" s="8">
+        <v>91939</v>
+      </c>
+      <c r="F140" s="8">
+        <v>54840</v>
+      </c>
+      <c r="G140" s="8">
+        <v>57813</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B141" s="7">
+        <v>905</v>
+      </c>
+      <c r="C141" s="4">
+        <v>5425</v>
+      </c>
+      <c r="D141" s="4">
+        <v>17169</v>
+      </c>
+      <c r="E141" s="4">
+        <v>74578</v>
+      </c>
+      <c r="F141" s="4">
+        <v>62669</v>
+      </c>
+      <c r="G141" s="4">
+        <v>125389</v>
+      </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
@@ -9403,6 +12476,16 @@
       <c r="H151" s="7" t="s">
         <v>37</v>
       </c>
+    </row>
+    <row r="166" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="M166" s="21"/>
+      <c r="N166" s="21"/>
+      <c r="O166" s="21"/>
+      <c r="P166" s="21"/>
+      <c r="Q166" s="21"/>
+      <c r="R166" s="21"/>
+      <c r="S166" s="21"/>
+      <c r="T166" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>